<commit_message>
Finished the annotation. BUT still need to check the [???] cases!!!
</commit_message>
<xml_diff>
--- a/SolrScripts/results-gc/set-verifying/verifying-set-felipe.xlsx
+++ b/SolrScripts/results-gc/set-verifying/verifying-set-felipe.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="904">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="915">
   <si>
     <t>id</t>
   </si>
@@ -3491,6 +3491,39 @@
   </si>
   <si>
     <t>The author is uncertain about the build's fail</t>
+  </si>
+  <si>
+    <t>The author is confused about the code</t>
+  </si>
+  <si>
+    <t>The author is uncertain about the usefulness of a part of the code</t>
+  </si>
+  <si>
+    <t>The author is uncertain about how to proceed with the code and also how it works</t>
+  </si>
+  <si>
+    <t>The author is uncertain about how something disappeared</t>
+  </si>
+  <si>
+    <t>The author is uncertain about the need of sanity checks</t>
+  </si>
+  <si>
+    <t>The author is confused about changes</t>
+  </si>
+  <si>
+    <t>The author is confused about the change's goal</t>
+  </si>
+  <si>
+    <t>The authos is confused about the chage's context</t>
+  </si>
+  <si>
+    <t>The author is uncertain about the need of opening dex files</t>
+  </si>
+  <si>
+    <t>The author is uncertain about his code</t>
+  </si>
+  <si>
+    <t>The author is uncertain abou the need of some libs</t>
   </si>
 </sst>
 </file>
@@ -3611,327 +3644,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4230,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B335" workbookViewId="0">
-      <selection activeCell="D341" sqref="D341"/>
+    <sheetView tabSelected="1" topLeftCell="B380" workbookViewId="0">
+      <selection activeCell="C381" sqref="C381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4239,7 +3952,7 @@
     <col min="1" max="1" width="43.44140625" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="103.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
+    <col min="4" max="4" width="70.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -8129,7 +7842,9 @@
       <c r="B341" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="C341" s="2"/>
+      <c r="C341" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="342" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
@@ -8138,7 +7853,9 @@
       <c r="B342" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="C342" s="2"/>
+      <c r="C342" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="343" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
@@ -8147,7 +7864,12 @@
       <c r="B343" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="C343" s="2"/>
+      <c r="C343" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D343" t="s">
+        <v>904</v>
+      </c>
     </row>
     <row r="344" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
@@ -8156,7 +7878,12 @@
       <c r="B344" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="C344" s="2"/>
+      <c r="C344" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="D344" t="s">
+        <v>897</v>
+      </c>
     </row>
     <row r="345" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
@@ -8165,7 +7892,9 @@
       <c r="B345" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="C345" s="2"/>
+      <c r="C345" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="346" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
@@ -8174,7 +7903,9 @@
       <c r="B346" s="4" t="s">
         <v>634</v>
       </c>
-      <c r="C346" s="2"/>
+      <c r="C346" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="347" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
@@ -8183,7 +7914,9 @@
       <c r="B347" s="4" t="s">
         <v>636</v>
       </c>
-      <c r="C347" s="2"/>
+      <c r="C347" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="348" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
@@ -8192,7 +7925,9 @@
       <c r="B348" s="4" t="s">
         <v>638</v>
       </c>
-      <c r="C348" s="2"/>
+      <c r="C348" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="349" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
@@ -8201,7 +7936,9 @@
       <c r="B349" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="C349" s="2"/>
+      <c r="C349" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="350" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
@@ -8210,7 +7947,12 @@
       <c r="B350" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="C350" s="2"/>
+      <c r="C350" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D350" t="s">
+        <v>888</v>
+      </c>
     </row>
     <row r="351" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
@@ -8219,7 +7961,9 @@
       <c r="B351" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="C351" s="2"/>
+      <c r="C351" s="2" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="352" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
@@ -8228,719 +7972,913 @@
       <c r="B352" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="C352" s="2"/>
-    </row>
-    <row r="353" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C352" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>647</v>
       </c>
       <c r="B353" s="4" t="s">
         <v>648</v>
       </c>
-      <c r="C353" s="2"/>
-    </row>
-    <row r="354" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C353" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>649</v>
       </c>
       <c r="B354" s="4" t="s">
         <v>650</v>
       </c>
-      <c r="C354" s="2"/>
-    </row>
-    <row r="355" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C354" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>651</v>
       </c>
       <c r="B355" s="4" t="s">
         <v>652</v>
       </c>
-      <c r="C355" s="2"/>
-    </row>
-    <row r="356" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C355" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>653</v>
       </c>
       <c r="B356" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="C356" s="2"/>
-    </row>
-    <row r="357" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C356" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>655</v>
       </c>
       <c r="B357" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="C357" s="2"/>
-    </row>
-    <row r="358" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C357" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>657</v>
       </c>
       <c r="B358" s="4" t="s">
         <v>658</v>
       </c>
-      <c r="C358" s="2"/>
-    </row>
-    <row r="359" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C358" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>659</v>
       </c>
       <c r="B359" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="C359" s="2"/>
-    </row>
-    <row r="360" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C359" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>661</v>
       </c>
       <c r="B360" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="C360" s="2"/>
-    </row>
-    <row r="361" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C360" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>663</v>
       </c>
       <c r="B361" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="C361" s="2"/>
-    </row>
-    <row r="362" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C361" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>665</v>
       </c>
       <c r="B362" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="C362" s="2"/>
-    </row>
-    <row r="363" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C362" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>667</v>
       </c>
       <c r="B363" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="C363" s="2"/>
-    </row>
-    <row r="364" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C363" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>669</v>
       </c>
       <c r="B364" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="C364" s="2"/>
-    </row>
-    <row r="365" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C364" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>671</v>
       </c>
       <c r="B365" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="C365" s="2"/>
-    </row>
-    <row r="366" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C365" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D365" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>673</v>
       </c>
       <c r="B366" s="4" t="s">
         <v>674</v>
       </c>
-      <c r="C366" s="2"/>
-    </row>
-    <row r="367" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C366" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>675</v>
       </c>
       <c r="B367" s="4" t="s">
         <v>676</v>
       </c>
-      <c r="C367" s="2"/>
-    </row>
-    <row r="368" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="C367" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>677</v>
       </c>
       <c r="B368" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="C368" s="2"/>
-    </row>
-    <row r="369" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C368" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D368" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>679</v>
       </c>
       <c r="B369" s="4" t="s">
         <v>680</v>
       </c>
-      <c r="C369" s="2"/>
-    </row>
-    <row r="370" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C369" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>681</v>
       </c>
       <c r="B370" s="4" t="s">
         <v>682</v>
       </c>
-      <c r="C370" s="2"/>
-    </row>
-    <row r="371" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C370" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>683</v>
       </c>
       <c r="B371" s="4" t="s">
         <v>684</v>
       </c>
-      <c r="C371" s="2"/>
-    </row>
-    <row r="372" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C371" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>685</v>
       </c>
       <c r="B372" s="4" t="s">
         <v>686</v>
       </c>
-      <c r="C372" s="2"/>
-    </row>
-    <row r="373" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C372" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D372" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>687</v>
       </c>
       <c r="B373" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="C373" s="2"/>
-    </row>
-    <row r="374" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C373" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>689</v>
       </c>
       <c r="B374" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="C374" s="2"/>
-    </row>
-    <row r="375" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C374" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>691</v>
       </c>
       <c r="B375" s="4" t="s">
         <v>692</v>
       </c>
-      <c r="C375" s="2"/>
-    </row>
-    <row r="376" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C375" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>693</v>
       </c>
       <c r="B376" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="C376" s="2"/>
-    </row>
-    <row r="377" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="C376" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>695</v>
       </c>
       <c r="B377" s="4" t="s">
         <v>696</v>
       </c>
-      <c r="C377" s="2"/>
-    </row>
-    <row r="378" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C377" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>697</v>
       </c>
       <c r="B378" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="C378" s="2"/>
-    </row>
-    <row r="379" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C378" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>699</v>
       </c>
       <c r="B379" s="4" t="s">
         <v>700</v>
       </c>
-      <c r="C379" s="2"/>
-    </row>
-    <row r="380" spans="1:3" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="C379" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>701</v>
       </c>
       <c r="B380" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="C380" s="2"/>
-    </row>
-    <row r="381" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C380" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>702</v>
       </c>
       <c r="B381" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="C381" s="2"/>
-    </row>
-    <row r="382" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="C381" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>704</v>
       </c>
       <c r="B382" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="C382" s="2"/>
-    </row>
-    <row r="383" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="C382" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>706</v>
       </c>
       <c r="B383" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="C383" s="2"/>
-    </row>
-    <row r="384" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="C383" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>708</v>
       </c>
       <c r="B384" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="C384" s="2"/>
-    </row>
-    <row r="385" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C384" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>710</v>
       </c>
       <c r="B385" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="C385" s="2"/>
-    </row>
-    <row r="386" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C385" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>712</v>
       </c>
       <c r="B386" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="C386" s="2"/>
-    </row>
-    <row r="387" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C386" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>714</v>
       </c>
       <c r="B387" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="C387" s="2"/>
-    </row>
-    <row r="388" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C387" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>716</v>
       </c>
       <c r="B388" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="C388" s="2"/>
-    </row>
-    <row r="389" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C388" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>718</v>
       </c>
       <c r="B389" s="4" t="s">
         <v>719</v>
       </c>
-      <c r="C389" s="2"/>
-    </row>
-    <row r="390" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="C389" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>720</v>
       </c>
       <c r="B390" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="C390" s="2"/>
-    </row>
-    <row r="391" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C390" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D390" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>722</v>
       </c>
       <c r="B391" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="C391" s="2"/>
-    </row>
-    <row r="392" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="C391" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>724</v>
       </c>
       <c r="B392" s="4" t="s">
         <v>725</v>
       </c>
-      <c r="C392" s="2"/>
-    </row>
-    <row r="393" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C392" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>726</v>
       </c>
       <c r="B393" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="C393" s="2"/>
-    </row>
-    <row r="394" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C393" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>728</v>
       </c>
       <c r="B394" s="4" t="s">
         <v>729</v>
       </c>
-      <c r="C394" s="2"/>
-    </row>
-    <row r="395" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="C394" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>730</v>
       </c>
       <c r="B395" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C395" s="2"/>
-    </row>
-    <row r="396" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="C395" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>731</v>
       </c>
       <c r="B396" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C396" s="2"/>
-    </row>
-    <row r="397" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C396" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>733</v>
       </c>
       <c r="B397" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="C397" s="2"/>
-    </row>
-    <row r="398" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C397" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>735</v>
       </c>
       <c r="B398" s="4" t="s">
         <v>736</v>
       </c>
-      <c r="C398" s="2"/>
-    </row>
-    <row r="399" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C398" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>737</v>
       </c>
       <c r="B399" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="C399" s="2"/>
-    </row>
-    <row r="400" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C399" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D399" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>739</v>
       </c>
       <c r="B400" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="C400" s="2"/>
-    </row>
-    <row r="401" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C400" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>741</v>
       </c>
       <c r="B401" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="C401" s="2"/>
-    </row>
-    <row r="402" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C401" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>743</v>
       </c>
       <c r="B402" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="C402" s="2"/>
-    </row>
-    <row r="403" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C402" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>745</v>
       </c>
       <c r="B403" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="C403" s="2"/>
-    </row>
-    <row r="404" spans="1:3" ht="171.6" x14ac:dyDescent="0.25">
+      <c r="C403" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>747</v>
       </c>
       <c r="B404" s="4" t="s">
         <v>748</v>
       </c>
-      <c r="C404" s="2"/>
-    </row>
-    <row r="405" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C404" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D404" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>749</v>
       </c>
       <c r="B405" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="C405" s="2"/>
-    </row>
-    <row r="406" spans="1:3" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="C405" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>751</v>
       </c>
       <c r="B406" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="C406" s="2"/>
-    </row>
-    <row r="407" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C406" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>753</v>
       </c>
       <c r="B407" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="C407" s="2"/>
-    </row>
-    <row r="408" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C407" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>755</v>
       </c>
       <c r="B408" s="4" t="s">
         <v>756</v>
       </c>
-      <c r="C408" s="2"/>
-    </row>
-    <row r="409" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="C408" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>757</v>
       </c>
       <c r="B409" s="4" t="s">
         <v>758</v>
       </c>
-      <c r="C409" s="2"/>
-    </row>
-    <row r="410" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C409" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D409" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>759</v>
       </c>
       <c r="B410" s="4" t="s">
         <v>760</v>
       </c>
-      <c r="C410" s="2"/>
-    </row>
-    <row r="411" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C410" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>761</v>
       </c>
       <c r="B411" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="C411" s="2"/>
-    </row>
-    <row r="412" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C411" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>763</v>
       </c>
       <c r="B412" s="4" t="s">
         <v>764</v>
       </c>
-      <c r="C412" s="2"/>
-    </row>
-    <row r="413" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C412" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>765</v>
       </c>
       <c r="B413" s="4" t="s">
         <v>766</v>
       </c>
-      <c r="C413" s="2"/>
-    </row>
-    <row r="414" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C413" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>767</v>
       </c>
       <c r="B414" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="C414" s="2"/>
-    </row>
-    <row r="415" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C414" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D414" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>769</v>
       </c>
       <c r="B415" s="4" t="s">
         <v>770</v>
       </c>
-      <c r="C415" s="2"/>
-    </row>
-    <row r="416" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C415" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D415" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>771</v>
       </c>
       <c r="B416" s="4" t="s">
         <v>772</v>
       </c>
-      <c r="C416" s="2"/>
-    </row>
-    <row r="417" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="C416" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>773</v>
       </c>
       <c r="B417" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="C417" s="2"/>
-    </row>
-    <row r="418" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C417" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>775</v>
       </c>
       <c r="B418" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="C418" s="2"/>
-    </row>
-    <row r="419" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C418" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D418" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>777</v>
       </c>
       <c r="B419" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="C419" s="2"/>
-    </row>
-    <row r="420" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C419" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>779</v>
       </c>
       <c r="B420" s="4" t="s">
         <v>780</v>
       </c>
-      <c r="C420" s="2"/>
-    </row>
-    <row r="421" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C420" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>781</v>
       </c>
       <c r="B421" s="4" t="s">
         <v>782</v>
       </c>
-      <c r="C421" s="2"/>
-    </row>
-    <row r="422" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="C421" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>783</v>
       </c>
       <c r="B422" s="4" t="s">
         <v>784</v>
       </c>
-      <c r="C422" s="2"/>
-    </row>
-    <row r="423" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C422" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D422" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>785</v>
       </c>
       <c r="B423" s="4" t="s">
         <v>786</v>
       </c>
-      <c r="C423" s="2"/>
-    </row>
-    <row r="424" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C423" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>787</v>
       </c>
       <c r="B424" s="4" t="s">
         <v>788</v>
       </c>
-      <c r="C424" s="2"/>
-    </row>
-    <row r="425" spans="1:3" ht="118.8" x14ac:dyDescent="0.25">
+      <c r="C424" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>789</v>
       </c>
       <c r="B425" s="4" t="s">
         <v>790</v>
       </c>
-      <c r="C425" s="2"/>
-    </row>
-    <row r="426" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C425" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>791</v>
       </c>
       <c r="B426" s="4" t="s">
         <v>792</v>
       </c>
-      <c r="C426" s="2"/>
-    </row>
-    <row r="427" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="C426" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>793</v>
       </c>
       <c r="B427" s="4" t="s">
         <v>794</v>
       </c>
-      <c r="C427" s="2"/>
-    </row>
-    <row r="428" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="C427" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>795</v>
       </c>
       <c r="B428" s="4" t="s">
         <v>796</v>
       </c>
-      <c r="C428" s="2"/>
-    </row>
-    <row r="429" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="C428" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>797</v>
       </c>
       <c r="B429" s="4" t="s">
         <v>798</v>
       </c>
-      <c r="C429" s="2"/>
-    </row>
-    <row r="430" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="C429" s="2" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" ht="66" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>799</v>
       </c>
       <c r="B430" s="4" t="s">
         <v>800</v>
       </c>
-      <c r="C430" s="2"/>
+      <c r="C430" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D430" t="s">
+        <v>908</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C27 B1 B28:B30 B431:B1048576 C31:C430">
-    <cfRule type="containsText" dxfId="33" priority="1" stopIfTrue="1" operator="containsText" text="no">
+    <cfRule type="containsText" dxfId="1" priority="1" stopIfTrue="1" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="2" stopIfTrue="1" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="0" priority="2" stopIfTrue="1" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>